<commit_message>
Added data from Solar Api Calls for first 60 locations - Amanda
</commit_message>
<xml_diff>
--- a/SolarApiLocations.xlsx
+++ b/SolarApiLocations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d353e6827118956a/addressToDistance/addressToExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="449" documentId="11_217FF8C2F712DE19CC611F02D8539FE741A2C757" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FC4EED3-5912-4793-9BE3-769FCD47C468}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="11_217FF8C2F712DE19CC611F02D8539FE741A2C757" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52580C58-8D2D-48BE-9620-0A6511D2871D}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1524" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="364">
-  <si>
-    <t>Geocoding API</t>
-  </si>
-  <si>
-    <t>Actual</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="367">
   <si>
     <t>Name</t>
   </si>
@@ -56,10 +50,10 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>% Error Lat</t>
-  </si>
-  <si>
-    <t>% Error Long</t>
+    <t>% Error Latitude</t>
+  </si>
+  <si>
+    <t>% Error Longitude</t>
   </si>
   <si>
     <t>DataVerificationFlag</t>
@@ -1128,16 +1122,39 @@
   </si>
   <si>
     <t>100 Centennial Olympic Park Dr, Atlanta, GA 30313</t>
+  </si>
+  <si>
+    <t>NumPanels</t>
+  </si>
+  <si>
+    <t>YearlyEnergy</t>
+  </si>
+  <si>
+    <t>SolarArea</t>
+  </si>
+  <si>
+    <t>https://www.itilog.com/</t>
+  </si>
+  <si>
+    <t>Google Maps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1160,16 +1177,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1502,62 +1524,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I182"/>
+  <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C181" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I182"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="23.69921875" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" customWidth="1"/>
+    <col min="3" max="3" width="11.09765625" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="9.09765625" customWidth="1"/>
+    <col min="7" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.45" customHeight="1">
-      <c r="C1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>362</v>
+      </c>
+      <c r="K2" t="s">
+        <v>363</v>
+      </c>
+      <c r="L2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>33.583208900000002</v>
@@ -1583,13 +1623,22 @@
         <f>IF(OR(G3 &gt; 0.1, H3 &gt; 0.1), "1", "0")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75">
+      <c r="J3">
+        <v>540</v>
+      </c>
+      <c r="K3">
+        <v>1581.8035</v>
+      </c>
+      <c r="L3">
+        <v>1060.3196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>33.763472</v>
@@ -1615,13 +1664,22 @@
         <f t="shared" ref="I4:I67" si="2">IF(OR(G4 &gt; 0.1, H4 &gt; 0.1), "1", "0")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75">
+      <c r="J4">
+        <v>248</v>
+      </c>
+      <c r="K4">
+        <v>1565.5939000000001</v>
+      </c>
+      <c r="L4">
+        <v>486.96159999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>33.815625500000003</v>
@@ -1647,13 +1705,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75">
+      <c r="J5">
+        <v>1036</v>
+      </c>
+      <c r="K5">
+        <v>1570.4747</v>
+      </c>
+      <c r="L5">
+        <v>2034.2428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>33.860467999999997</v>
@@ -1679,13 +1746,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75">
+      <c r="J6">
+        <v>63</v>
+      </c>
+      <c r="K6">
+        <v>1484.3893</v>
+      </c>
+      <c r="L6">
+        <v>123.70396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>33.764702999999997</v>
@@ -1711,13 +1787,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75">
+      <c r="J7">
+        <v>165</v>
+      </c>
+      <c r="K7">
+        <v>1514.9232999999999</v>
+      </c>
+      <c r="L7">
+        <v>323.98653999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>34.215147100000003</v>
@@ -1743,13 +1828,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75">
+      <c r="J8">
+        <v>28</v>
+      </c>
+      <c r="K8">
+        <v>1549.3539000000001</v>
+      </c>
+      <c r="L8">
+        <v>54.979537999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>33.7545</v>
@@ -1775,13 +1869,22 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75">
+      <c r="J9">
+        <v>39</v>
+      </c>
+      <c r="K9">
+        <v>1624.2345</v>
+      </c>
+      <c r="L9">
+        <v>76.578636000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>33.846456000000003</v>
@@ -1807,13 +1910,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75">
+      <c r="J10">
+        <v>58</v>
+      </c>
+      <c r="K10">
+        <v>1386.1279</v>
+      </c>
+      <c r="L10">
+        <v>113.886185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>33.796058700000003</v>
@@ -1839,13 +1951,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75">
+      <c r="J11">
+        <v>405</v>
+      </c>
+      <c r="K11">
+        <v>1476.2083</v>
+      </c>
+      <c r="L11">
+        <v>795.23974999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>33.954263599999997</v>
@@ -1871,13 +1992,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75">
+      <c r="J12">
+        <v>642</v>
+      </c>
+      <c r="K12">
+        <v>1622.5833</v>
+      </c>
+      <c r="L12">
+        <v>1260.6022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>33.725418300000001</v>
@@ -1903,13 +2033,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75">
+      <c r="J13">
+        <v>370</v>
+      </c>
+      <c r="K13">
+        <v>1570.1890000000001</v>
+      </c>
+      <c r="L13">
+        <v>726.51530000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>33.772438600000001</v>
@@ -1935,13 +2074,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75">
+      <c r="J14">
+        <v>4530</v>
+      </c>
+      <c r="K14">
+        <v>1612.1111000000001</v>
+      </c>
+      <c r="L14">
+        <v>8894.9030000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>33.722366999999998</v>
@@ -1967,13 +2115,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75">
+      <c r="J15">
+        <v>66</v>
+      </c>
+      <c r="K15">
+        <v>1563.7988</v>
+      </c>
+      <c r="L15">
+        <v>129.7988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>33.630500400000003</v>
@@ -1999,13 +2156,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75">
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="K16">
+        <v>1645.4679000000001</v>
+      </c>
+      <c r="L16">
+        <v>49.08887</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>33.807581999999996</v>
@@ -2031,13 +2197,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75">
+      <c r="J17">
+        <v>442</v>
+      </c>
+      <c r="K17">
+        <v>1498.6993</v>
+      </c>
+      <c r="L17">
+        <v>867.89124000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>33.740336499999998</v>
@@ -2063,13 +2238,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75">
+      <c r="J18">
+        <v>57</v>
+      </c>
+      <c r="K18">
+        <v>1478.6083000000001</v>
+      </c>
+      <c r="L18">
+        <v>111.92263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>33.659350199999999</v>
@@ -2095,13 +2279,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75">
+      <c r="J19">
+        <v>306</v>
+      </c>
+      <c r="K19">
+        <v>1682.5786000000001</v>
+      </c>
+      <c r="L19">
+        <v>600.84780000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>33.772683999999998</v>
@@ -2127,13 +2320,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75">
+      <c r="J20">
+        <v>51</v>
+      </c>
+      <c r="K20">
+        <v>1549.7965999999999</v>
+      </c>
+      <c r="L20">
+        <v>100.1413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>33.772509399999997</v>
@@ -2159,13 +2361,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75">
+      <c r="J21">
+        <v>487</v>
+      </c>
+      <c r="K21">
+        <v>1590.6071999999999</v>
+      </c>
+      <c r="L21">
+        <v>956.25120000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>33.749718600000001</v>
@@ -2191,13 +2402,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75">
+      <c r="J22">
+        <v>1270</v>
+      </c>
+      <c r="K22">
+        <v>1677.4454000000001</v>
+      </c>
+      <c r="L22">
+        <v>2493.7145999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>33.452597900000001</v>
@@ -2223,13 +2443,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75">
+      <c r="J23">
+        <v>174</v>
+      </c>
+      <c r="K23">
+        <v>1468.0625</v>
+      </c>
+      <c r="L23">
+        <v>341.65854000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>33.929813699999997</v>
@@ -2255,13 +2484,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75">
+      <c r="J24">
+        <v>263</v>
+      </c>
+      <c r="K24">
+        <v>1562.1947</v>
+      </c>
+      <c r="L24">
+        <v>516.41489999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>33.798876999999997</v>
@@ -2287,13 +2525,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75">
+      <c r="J25">
+        <v>33</v>
+      </c>
+      <c r="K25">
+        <v>1387.6632999999999</v>
+      </c>
+      <c r="L25">
+        <v>64.797309999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26">
         <v>33.658856999999998</v>
@@ -2319,13 +2566,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75">
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26">
+        <v>1584.5623000000001</v>
+      </c>
+      <c r="L26">
+        <v>58.906647</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C27">
         <v>33.738007699999997</v>
@@ -2351,13 +2607,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75">
+      <c r="J27">
+        <v>51</v>
+      </c>
+      <c r="K27">
+        <v>1609.2815000000001</v>
+      </c>
+      <c r="L27">
+        <v>100.1413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28">
         <v>33.437151</v>
@@ -2383,13 +2648,22 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75">
+      <c r="J28">
+        <v>196</v>
+      </c>
+      <c r="K28">
+        <v>1584.2260000000001</v>
+      </c>
+      <c r="L28">
+        <v>384.85674999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29">
         <v>32.812421100000002</v>
@@ -2415,13 +2689,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75">
+      <c r="J29">
+        <v>46</v>
+      </c>
+      <c r="K29">
+        <v>1661.1687999999999</v>
+      </c>
+      <c r="L29">
+        <v>90.323524000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30">
         <v>33.740700699999998</v>
@@ -2447,13 +2730,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75">
+      <c r="J30">
+        <v>73</v>
+      </c>
+      <c r="K30">
+        <v>1663.7739999999999</v>
+      </c>
+      <c r="L30">
+        <v>143.33950999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31">
         <v>33.815027000000001</v>
@@ -2479,13 +2771,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75">
+      <c r="J31">
+        <v>115</v>
+      </c>
+      <c r="K31">
+        <v>1584.9971</v>
+      </c>
+      <c r="L31">
+        <v>225.80879999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32">
         <v>32.137238600000003</v>
@@ -2511,13 +2812,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75">
+      <c r="J32">
+        <v>822</v>
+      </c>
+      <c r="K32">
+        <v>1576.8373999999999</v>
+      </c>
+      <c r="L32">
+        <v>1614.0420999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C33">
         <v>33.810964300000002</v>
@@ -2543,13 +2853,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75">
+      <c r="J33">
+        <v>104</v>
+      </c>
+      <c r="K33">
+        <v>1665.7626</v>
+      </c>
+      <c r="L33">
+        <v>204.2097</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C34">
         <v>33.832065999999998</v>
@@ -2575,13 +2894,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75">
+      <c r="J34">
+        <v>212</v>
+      </c>
+      <c r="K34">
+        <v>1570.9668999999999</v>
+      </c>
+      <c r="L34">
+        <v>416.27361999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35">
         <v>33.747126299999998</v>
@@ -2607,13 +2935,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75">
+      <c r="J35">
+        <v>58</v>
+      </c>
+      <c r="K35">
+        <v>1584.8844999999999</v>
+      </c>
+      <c r="L35">
+        <v>113.886185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C36">
         <v>33.566949600000001</v>
@@ -2639,13 +2976,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75">
+      <c r="J36">
+        <v>144</v>
+      </c>
+      <c r="K36">
+        <v>1698.2602999999999</v>
+      </c>
+      <c r="L36">
+        <v>282.75189999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37">
         <v>33.98236</v>
@@ -2671,13 +3017,22 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75">
+      <c r="J37">
+        <v>59</v>
+      </c>
+      <c r="K37">
+        <v>1630.7167999999999</v>
+      </c>
+      <c r="L37">
+        <v>115.84974</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C38">
         <v>33.808487399999997</v>
@@ -2703,13 +3058,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75">
+      <c r="J38">
+        <v>858</v>
+      </c>
+      <c r="K38">
+        <v>1588.1403</v>
+      </c>
+      <c r="L38">
+        <v>1684.7301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39">
         <v>33.837895500000002</v>
@@ -2735,13 +3099,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75">
+      <c r="J39">
+        <v>159</v>
+      </c>
+      <c r="K39">
+        <v>1659.2025000000001</v>
+      </c>
+      <c r="L39">
+        <v>312.20522999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40">
         <v>33.817645800000001</v>
@@ -2767,13 +3140,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75">
+      <c r="J40">
+        <v>158</v>
+      </c>
+      <c r="K40">
+        <v>1492.2592999999999</v>
+      </c>
+      <c r="L40">
+        <v>310.24167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C41">
         <v>33.903649000000001</v>
@@ -2799,13 +3181,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75">
+      <c r="J41">
+        <v>711</v>
+      </c>
+      <c r="K41">
+        <v>1597.864</v>
+      </c>
+      <c r="L41">
+        <v>1396.0875000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C42">
         <v>33.798488999999996</v>
@@ -2831,13 +3222,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75">
+      <c r="J42">
+        <v>54</v>
+      </c>
+      <c r="K42">
+        <v>1570.1763000000001</v>
+      </c>
+      <c r="L42">
+        <v>106.03196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C43">
         <v>33.715308</v>
@@ -2863,13 +3263,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75">
+      <c r="J43">
+        <v>784</v>
+      </c>
+      <c r="K43">
+        <v>1577.2775999999999</v>
+      </c>
+      <c r="L43">
+        <v>1539.4269999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C44">
         <v>33.735278600000001</v>
@@ -2895,13 +3304,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75">
+      <c r="J44">
+        <v>33</v>
+      </c>
+      <c r="K44">
+        <v>1607.3677</v>
+      </c>
+      <c r="L44">
+        <v>64.797309999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C45">
         <v>33.745860299999997</v>
@@ -2927,13 +3345,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75">
+      <c r="J45">
+        <v>64</v>
+      </c>
+      <c r="K45">
+        <v>1595.9052999999999</v>
+      </c>
+      <c r="L45">
+        <v>125.66750999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46">
         <v>33.571651799999998</v>
@@ -2959,13 +3386,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75">
+      <c r="J46">
+        <v>187</v>
+      </c>
+      <c r="K46">
+        <v>1646.7550000000001</v>
+      </c>
+      <c r="L46">
+        <v>367.18475000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C47">
         <v>33.765948999999999</v>
@@ -2991,13 +3427,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75">
+      <c r="J47">
+        <v>159</v>
+      </c>
+      <c r="K47">
+        <v>1492.0681999999999</v>
+      </c>
+      <c r="L47">
+        <v>312.20522999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C48">
         <v>33.754370000000002</v>
@@ -3023,13 +3468,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75">
+      <c r="J48">
+        <v>62</v>
+      </c>
+      <c r="K48">
+        <v>1606.7845</v>
+      </c>
+      <c r="L48">
+        <v>121.74039999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C49">
         <v>34.086810300000003</v>
@@ -3055,13 +3509,22 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.75">
+      <c r="J49">
+        <v>515</v>
+      </c>
+      <c r="K49">
+        <v>1613.1375</v>
+      </c>
+      <c r="L49">
+        <v>1011.2308</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50">
         <v>33.738905000000003</v>
@@ -3087,13 +3550,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75">
+      <c r="J50">
+        <v>75</v>
+      </c>
+      <c r="K50">
+        <v>1562.2782</v>
+      </c>
+      <c r="L50">
+        <v>147.26661999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C51">
         <v>33.687238000000001</v>
@@ -3119,13 +3591,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75">
+      <c r="J51">
+        <v>62</v>
+      </c>
+      <c r="K51">
+        <v>1290.4568999999999</v>
+      </c>
+      <c r="L51">
+        <v>121.74039999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C52">
         <v>33.7267048</v>
@@ -3151,13 +3632,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75">
+      <c r="J52">
+        <v>27</v>
+      </c>
+      <c r="K52">
+        <v>1530.816</v>
+      </c>
+      <c r="L52">
+        <v>53.015979999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C53">
         <v>32.042782000000003</v>
@@ -3183,13 +3673,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.75">
+      <c r="J53">
+        <v>77</v>
+      </c>
+      <c r="K53">
+        <v>1658.4258</v>
+      </c>
+      <c r="L53">
+        <v>151.19372999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54">
         <v>33.805816999999998</v>
@@ -3215,13 +3714,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.75">
+      <c r="J54">
+        <v>73</v>
+      </c>
+      <c r="K54">
+        <v>1654.8463999999999</v>
+      </c>
+      <c r="L54">
+        <v>143.33950999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C55">
         <v>33.724860200000002</v>
@@ -3247,13 +3755,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75">
+      <c r="J55">
+        <v>3527</v>
+      </c>
+      <c r="K55">
+        <v>1575.4855</v>
+      </c>
+      <c r="L55">
+        <v>6925.4579999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C56">
         <v>33.857693900000001</v>
@@ -3279,13 +3796,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.75">
+      <c r="J56">
+        <v>38</v>
+      </c>
+      <c r="K56">
+        <v>1644.3524</v>
+      </c>
+      <c r="L56">
+        <v>74.615080000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C57">
         <v>33.717010299999998</v>
@@ -3311,13 +3837,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75">
+      <c r="J57">
+        <v>156</v>
+      </c>
+      <c r="K57">
+        <v>1489.527</v>
+      </c>
+      <c r="L57">
+        <v>306.31454000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C58">
         <v>33.877401999999996</v>
@@ -3343,13 +3878,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75">
+      <c r="J58">
+        <v>685</v>
+      </c>
+      <c r="K58">
+        <v>1573.2428</v>
+      </c>
+      <c r="L58">
+        <v>1345.0350000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C59">
         <v>33.737139399999997</v>
@@ -3375,13 +3919,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75">
+      <c r="J59">
+        <v>9</v>
+      </c>
+      <c r="K59">
+        <v>1683.2267999999999</v>
+      </c>
+      <c r="L59">
+        <v>17.671993000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C60">
         <v>33.815686200000002</v>
@@ -3407,13 +3960,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.75">
+      <c r="J60">
+        <v>91</v>
+      </c>
+      <c r="K60">
+        <v>1548.1699000000001</v>
+      </c>
+      <c r="L60">
+        <v>178.68349000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C61">
         <v>33.7402333</v>
@@ -3439,13 +4001,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15.75">
+      <c r="J61">
+        <v>41</v>
+      </c>
+      <c r="K61">
+        <v>1385.9257</v>
+      </c>
+      <c r="L61">
+        <v>80.505750000000006</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C62">
         <v>33.968812999999997</v>
@@ -3471,13 +4042,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.75">
+      <c r="J62">
+        <v>502</v>
+      </c>
+      <c r="K62">
+        <v>1609.6538</v>
+      </c>
+      <c r="L62">
+        <v>985.70450000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C63">
         <v>33.703305</v>
@@ -3504,12 +4084,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C64">
         <v>33.914669000000004</v>
@@ -3536,12 +4116,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.75">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C65">
         <v>33.950448000000002</v>
@@ -3568,12 +4148,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.75">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C66">
         <v>33.949232000000002</v>
@@ -3600,12 +4180,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.75">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C67">
         <v>33.721770499999998</v>
@@ -3632,12 +4212,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.75">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C68">
         <v>33.721167100000002</v>
@@ -3664,12 +4244,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.75">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C69">
         <v>33.739083700000002</v>
@@ -3696,12 +4276,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.75">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C70">
         <v>33.968812999999997</v>
@@ -3728,12 +4308,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.75">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C71">
         <v>33.7545</v>
@@ -3760,12 +4340,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.75">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C72">
         <v>33.8249657</v>
@@ -3792,12 +4372,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15.75">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C73">
         <v>33.939473999999997</v>
@@ -3824,12 +4404,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.75">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C74">
         <v>33.9907349</v>
@@ -3856,12 +4436,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.75">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C75">
         <v>33.773130999999999</v>
@@ -3888,12 +4468,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.75">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C76">
         <v>33.843772000000001</v>
@@ -3920,12 +4500,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.75">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C77">
         <v>33.781041100000003</v>
@@ -3952,12 +4532,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.75">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C78">
         <v>33.751421999999998</v>
@@ -3984,12 +4564,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15.75">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C79">
         <v>33.6592275</v>
@@ -4016,12 +4596,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.75">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C80">
         <v>33.754952000000003</v>
@@ -4048,12 +4628,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.75">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C81">
         <v>33.717010299999998</v>
@@ -4080,12 +4660,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.75">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B82" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C82">
         <v>33.610787899999998</v>
@@ -4112,12 +4692,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C83">
         <v>33.791340300000002</v>
@@ -4144,12 +4724,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.75">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B84" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C84">
         <v>33.782004399999998</v>
@@ -4176,12 +4756,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.75">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C85">
         <v>33.7557148</v>
@@ -4208,12 +4788,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.75">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C86">
         <v>33.79851</v>
@@ -4240,12 +4820,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.75">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B87" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C87">
         <v>33.755714500000003</v>
@@ -4272,12 +4852,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.75">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C88">
         <v>33.754415000000002</v>
@@ -4304,12 +4884,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.75">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B89" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C89">
         <v>33.772835700000002</v>
@@ -4336,12 +4916,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.75">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B90" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C90">
         <v>33.841368799999998</v>
@@ -4368,12 +4948,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15.75">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B91" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C91">
         <v>33.665668699999998</v>
@@ -4400,12 +4980,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15.75">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B92" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C92">
         <v>33.799787999999999</v>
@@ -4432,12 +5012,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15.75">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C93">
         <v>33.754341500000002</v>
@@ -4464,12 +5044,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.75">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C94">
         <v>32.115523000000003</v>
@@ -4496,12 +5076,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15.75">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B95" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C95">
         <v>33.781992199999998</v>
@@ -4528,12 +5108,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15.75">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B96" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C96">
         <v>33.798876999999997</v>
@@ -4560,12 +5140,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15.75">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B97" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C97">
         <v>33.793464399999998</v>
@@ -4592,12 +5172,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15.75">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B98" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C98">
         <v>33.747302599999998</v>
@@ -4624,12 +5204,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.75">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B99" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C99">
         <v>33.711010799999997</v>
@@ -4656,12 +5236,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.75">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B100" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C100">
         <v>33.451042999999999</v>
@@ -4688,12 +5268,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.75">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B101" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C101">
         <v>32.056704600000003</v>
@@ -4720,12 +5300,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.75">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B102" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C102">
         <v>33.800682999999999</v>
@@ -4752,12 +5332,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15.75">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B103" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C103">
         <v>33.774882400000003</v>
@@ -4784,12 +5364,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.75">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B104" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C104">
         <v>33.894237099999998</v>
@@ -4816,12 +5396,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.75">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B105" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C105">
         <v>33.653679799999999</v>
@@ -4848,12 +5428,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15.75">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B106" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C106">
         <v>33.796058700000003</v>
@@ -4880,12 +5460,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.75">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C107">
         <v>33.749661500000002</v>
@@ -4912,12 +5492,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15.75">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B108" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C108">
         <v>32.824657000000002</v>
@@ -4944,12 +5524,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.75">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B109" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C109">
         <v>33.815211300000001</v>
@@ -4976,12 +5556,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.75">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B110" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C110">
         <v>33.749476999999999</v>
@@ -5008,12 +5588,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15.75">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B111" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C111">
         <v>33.6581422</v>
@@ -5040,12 +5620,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15.75">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B112" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C112">
         <v>33.774410699999997</v>
@@ -5072,12 +5652,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15.75">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B113" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C113">
         <v>33.738393000000002</v>
@@ -5104,12 +5684,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.75">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B114" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C114">
         <v>33.775718699999999</v>
@@ -5136,12 +5716,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15.75">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B115" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C115">
         <v>33.738534999999999</v>
@@ -5168,12 +5748,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15.75">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B116" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C116">
         <v>33.951830299999997</v>
@@ -5200,12 +5780,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15.75">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B117" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C117">
         <v>33.752575</v>
@@ -5232,12 +5812,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15.75">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B118" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C118">
         <v>33.640806099999999</v>
@@ -5264,12 +5844,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="15.75">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B119" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C119">
         <v>33.795105999999997</v>
@@ -5296,12 +5876,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="15.75">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B120" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C120">
         <v>33.7549511</v>
@@ -5328,12 +5908,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="15.75">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B121" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C121">
         <v>33.876629000000001</v>
@@ -5360,12 +5940,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="15.75">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B122" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C122">
         <v>33.777293</v>
@@ -5392,12 +5972,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="15.75">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B123" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C123">
         <v>33.892690000000002</v>
@@ -5424,12 +6004,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="15.75">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B124" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C124">
         <v>33.889257999999998</v>
@@ -5456,12 +6036,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15.75">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B125" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C125">
         <v>33.6514588</v>
@@ -5488,12 +6068,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.75">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B126" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C126">
         <v>33.690572000000003</v>
@@ -5520,12 +6100,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15.75">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B127" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C127">
         <v>33.774882400000003</v>
@@ -5552,12 +6132,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.75">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B128" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C128">
         <v>33.739026799999998</v>
@@ -5584,12 +6164,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="15.75">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B129" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C129">
         <v>33.754378000000003</v>
@@ -5616,12 +6196,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="15.75">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>256</v>
+      </c>
+      <c r="B130" t="s">
         <v>258</v>
-      </c>
-      <c r="B130" t="s">
-        <v>260</v>
       </c>
       <c r="C130">
         <v>33.525095999999998</v>
@@ -5648,12 +6228,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="15.75">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B131" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C131">
         <v>34.0066214</v>
@@ -5680,12 +6260,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="15.75">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B132" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C132">
         <v>33.743516</v>
@@ -5708,16 +6288,16 @@
         <v>6.6712643073915944E-5</v>
       </c>
       <c r="I132" t="str">
-        <f t="shared" ref="I132:I182" si="8">IF(OR(G132 &gt; 0.1, H132 &gt; 0.1), "1", "0")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.75">
+        <f t="shared" ref="I132:I181" si="8">IF(OR(G132 &gt; 0.1, H132 &gt; 0.1), "1", "0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B133" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C133">
         <v>33.772205399999997</v>
@@ -5744,12 +6324,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="15.75">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B134" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C134">
         <v>33.738167799999999</v>
@@ -5776,12 +6356,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="15.75">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B135" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C135">
         <v>33.876629000000001</v>
@@ -5808,12 +6388,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15.75">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B136" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C136">
         <v>33.886471999999998</v>
@@ -5840,12 +6420,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="15.75">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B137" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C137">
         <v>33.736809000000001</v>
@@ -5872,12 +6452,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.75">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B138" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C138">
         <v>33.747542000000003</v>
@@ -5904,12 +6484,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15.75">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B139" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C139">
         <v>33.472682599999999</v>
@@ -5936,12 +6516,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15.75">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B140" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C140">
         <v>33.781856400000002</v>
@@ -5968,12 +6548,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15.75">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>277</v>
+      </c>
+      <c r="B141" t="s">
         <v>279</v>
-      </c>
-      <c r="B141" t="s">
-        <v>281</v>
       </c>
       <c r="C141">
         <v>33.8284533</v>
@@ -6000,12 +6580,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="15.75">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B142" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C142">
         <v>33.531801000000002</v>
@@ -6032,12 +6612,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15.75">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B143" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C143">
         <v>33.583321099999999</v>
@@ -6064,12 +6644,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="15.75">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B144" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C144">
         <v>33.750441799999997</v>
@@ -6096,12 +6676,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="15.75">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B145" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C145">
         <v>33.738387400000001</v>
@@ -6128,12 +6708,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="15.75">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B146" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C146">
         <v>33.773077000000001</v>
@@ -6160,12 +6740,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15.75">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B147" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C147">
         <v>33.740399099999998</v>
@@ -6192,12 +6772,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15.75">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B148" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C148">
         <v>33.800226000000002</v>
@@ -6224,12 +6804,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15.75">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B149" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C149">
         <v>33.722276600000001</v>
@@ -6256,12 +6836,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15.75">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B150" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C150">
         <v>33.740657200000001</v>
@@ -6288,12 +6868,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="15.75">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B151" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C151">
         <v>33.945991999999997</v>
@@ -6320,12 +6900,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15.75">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B152" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C152">
         <v>33.754531</v>
@@ -6352,12 +6932,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="15.75">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B153" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C153">
         <v>33.663263899999997</v>
@@ -6384,12 +6964,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="15.75">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B154" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C154">
         <v>33.781421299999998</v>
@@ -6416,12 +6996,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="15.75">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B155" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C155">
         <v>33.650859400000002</v>
@@ -6448,12 +7028,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="15.75">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B156" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C156">
         <v>33.758375299999997</v>
@@ -6480,12 +7060,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="15.75">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B157" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C157">
         <v>33.7859281</v>
@@ -6512,12 +7092,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.75">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B158" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C158">
         <v>33.810287700000003</v>
@@ -6544,12 +7124,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="15.75">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B159" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C159">
         <v>33.809074000000003</v>
@@ -6576,12 +7156,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="15.75">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B160" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C160">
         <v>33.755504299999998</v>
@@ -6608,12 +7188,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="15.75">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B161" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C161">
         <v>33.602426999999999</v>
@@ -6640,12 +7220,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="15.75">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B162" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C162">
         <v>33.484462000000001</v>
@@ -6672,12 +7252,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="15.75">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B163" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C163">
         <v>33.653759399999998</v>
@@ -6704,12 +7284,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="15.75">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B164" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C164">
         <v>33.767305999999998</v>
@@ -6736,12 +7316,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="15.75">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B165" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C165">
         <v>33.826422999999998</v>
@@ -6768,12 +7348,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="15.75">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B166" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C166">
         <v>33.746398999999997</v>
@@ -6800,12 +7380,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="15.75">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B167" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C167">
         <v>33.7865605</v>
@@ -6832,12 +7412,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="15.75">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B168" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C168">
         <v>33.807989999999997</v>
@@ -6864,12 +7444,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.75">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B169" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C169">
         <v>33.651388300000001</v>
@@ -6896,12 +7476,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="15.75">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B170" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C170">
         <v>33.782835599999999</v>
@@ -6928,12 +7508,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="15.75">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B171" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C171">
         <v>33.777701800000003</v>
@@ -6960,12 +7540,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="15.75">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B172" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C172">
         <v>33.7395864</v>
@@ -6992,12 +7572,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="15.75">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B173" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C173">
         <v>33.923588000000002</v>
@@ -7024,12 +7604,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="15.75">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B174" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C174">
         <v>33.774696400000003</v>
@@ -7056,12 +7636,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="15.75">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B175" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C175">
         <v>33.680609699999998</v>
@@ -7088,12 +7668,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="15.75">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B176" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C176">
         <v>33.9585376</v>
@@ -7120,12 +7700,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="15.75">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B177" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C177">
         <v>33.950010599999999</v>
@@ -7152,12 +7732,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="15.75">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B178" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C178">
         <v>33.550077000000002</v>
@@ -7184,12 +7764,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="15.75">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B179" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C179">
         <v>33.6102116</v>
@@ -7216,12 +7796,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="15.75">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B180" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C180">
         <v>33.859588000000002</v>
@@ -7248,12 +7828,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="15.75">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B181" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C181">
         <v>33.846677</v>
@@ -7280,12 +7860,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="15.75">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B182" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C182">
         <v>33.765948999999999</v>
@@ -7308,7 +7888,7 @@
         <v>8.3535855048135974E-3</v>
       </c>
       <c r="I182" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(OR(G182 &gt; 0.1, H182 &gt; 0.1), "1", "0")</f>
         <v>0</v>
       </c>
     </row>
@@ -7317,9 +7897,12 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{83DA0028-B68A-41AF-B62F-8192A62EA8BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:D2 A7:D55 D3 B4:D4 B5:D5 A6:B6 D6 A57:D64 A56 C56:D56 A66:D99 B65:D65 A154:D182 B153:D153 A101:D152 B100:D100" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:D2 A7:D55 D3 B4:D4 B5:D5 A6:B6 D6 A57:D64 A56 C56:D56 A66:D99 B65:D65 A154:D178 B153:D153 A101:D152 B100:D100 A180:D182 B179:D179" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed YearlyEnergy Data - Amanda
</commit_message>
<xml_diff>
--- a/SolarApiLocations.xlsx
+++ b/SolarApiLocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d353e6827118956a/addressToDistance/addressToExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="502" documentId="11_217FF8C2F712DE19CC611F02D8539FE741A2C757" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52580C58-8D2D-48BE-9620-0A6511D2871D}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="11_217FF8C2F712DE19CC611F02D8539FE741A2C757" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CC09D75-EAD3-4B4E-A09F-8C6B254AE905}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1627,7 +1627,7 @@
         <v>540</v>
       </c>
       <c r="K3">
-        <v>1581.8035</v>
+        <v>333510.13</v>
       </c>
       <c r="L3">
         <v>1060.3196</v>
@@ -1668,7 +1668,7 @@
         <v>248</v>
       </c>
       <c r="K4">
-        <v>1565.5939000000001</v>
+        <v>144010.17000000001</v>
       </c>
       <c r="L4">
         <v>486.96159999999998</v>
@@ -1709,7 +1709,7 @@
         <v>1036</v>
       </c>
       <c r="K5">
-        <v>1570.4747</v>
+        <v>568353.80000000005</v>
       </c>
       <c r="L5">
         <v>2034.2428</v>
@@ -1750,7 +1750,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>1484.3893</v>
+        <v>31969.133000000002</v>
       </c>
       <c r="L6">
         <v>123.70396</v>
@@ -1791,7 +1791,7 @@
         <v>165</v>
       </c>
       <c r="K7">
-        <v>1514.9232999999999</v>
+        <v>95746.48</v>
       </c>
       <c r="L7">
         <v>323.98653999999999</v>
@@ -1832,7 +1832,7 @@
         <v>28</v>
       </c>
       <c r="K8">
-        <v>1549.3539000000001</v>
+        <v>16722.208999999999</v>
       </c>
       <c r="L8">
         <v>54.979537999999998</v>
@@ -1873,7 +1873,7 @@
         <v>39</v>
       </c>
       <c r="K9">
-        <v>1624.2345</v>
+        <v>20176.07</v>
       </c>
       <c r="L9">
         <v>76.578636000000003</v>
@@ -1914,7 +1914,7 @@
         <v>58</v>
       </c>
       <c r="K10">
-        <v>1386.1279</v>
+        <v>27227.153999999999</v>
       </c>
       <c r="L10">
         <v>113.886185</v>
@@ -1955,7 +1955,7 @@
         <v>405</v>
       </c>
       <c r="K11">
-        <v>1476.2083</v>
+        <v>206903.03</v>
       </c>
       <c r="L11">
         <v>795.23974999999996</v>
@@ -1996,7 +1996,7 @@
         <v>642</v>
       </c>
       <c r="K12">
-        <v>1622.5833</v>
+        <v>377165</v>
       </c>
       <c r="L12">
         <v>1260.6022</v>
@@ -2037,7 +2037,7 @@
         <v>370</v>
       </c>
       <c r="K13">
-        <v>1570.1890000000001</v>
+        <v>217364.14</v>
       </c>
       <c r="L13">
         <v>726.51530000000002</v>
@@ -2078,7 +2078,7 @@
         <v>4530</v>
       </c>
       <c r="K14">
-        <v>1612.1111000000001</v>
+        <v>2501681.5</v>
       </c>
       <c r="L14">
         <v>8894.9030000000002</v>
@@ -2119,7 +2119,7 @@
         <v>66</v>
       </c>
       <c r="K15">
-        <v>1563.7988</v>
+        <v>38155.207000000002</v>
       </c>
       <c r="L15">
         <v>129.7988</v>
@@ -2160,7 +2160,7 @@
         <v>25</v>
       </c>
       <c r="K16">
-        <v>1645.4679000000001</v>
+        <v>15053.463</v>
       </c>
       <c r="L16">
         <v>49.08887</v>
@@ -2201,7 +2201,7 @@
         <v>442</v>
       </c>
       <c r="K17">
-        <v>1498.6993</v>
+        <v>251645.22</v>
       </c>
       <c r="L17">
         <v>867.89124000000004</v>
@@ -2242,7 +2242,7 @@
         <v>57</v>
       </c>
       <c r="K18">
-        <v>1478.6083000000001</v>
+        <v>31206.947</v>
       </c>
       <c r="L18">
         <v>111.92263</v>
@@ -2283,7 +2283,7 @@
         <v>306</v>
       </c>
       <c r="K19">
-        <v>1682.5786000000001</v>
+        <v>178301.69</v>
       </c>
       <c r="L19">
         <v>600.84780000000001</v>
@@ -2324,7 +2324,7 @@
         <v>51</v>
       </c>
       <c r="K20">
-        <v>1549.7965999999999</v>
+        <v>27977.474999999999</v>
       </c>
       <c r="L20">
         <v>100.1413</v>
@@ -2365,7 +2365,7 @@
         <v>487</v>
       </c>
       <c r="K21">
-        <v>1590.6071999999999</v>
+        <v>275806.13</v>
       </c>
       <c r="L21">
         <v>956.25120000000004</v>
@@ -2406,7 +2406,7 @@
         <v>1270</v>
       </c>
       <c r="K22">
-        <v>1677.4454000000001</v>
+        <v>676217.25</v>
       </c>
       <c r="L22">
         <v>2493.7145999999998</v>
@@ -2447,7 +2447,7 @@
         <v>174</v>
       </c>
       <c r="K23">
-        <v>1468.0625</v>
+        <v>75689.97</v>
       </c>
       <c r="L23">
         <v>341.65854000000002</v>
@@ -2488,7 +2488,7 @@
         <v>263</v>
       </c>
       <c r="K24">
-        <v>1562.1947</v>
+        <v>151941.29999999999</v>
       </c>
       <c r="L24">
         <v>516.41489999999999</v>
@@ -2529,7 +2529,7 @@
         <v>33</v>
       </c>
       <c r="K25">
-        <v>1387.6632999999999</v>
+        <v>14786.965</v>
       </c>
       <c r="L25">
         <v>64.797309999999996</v>
@@ -2570,7 +2570,7 @@
         <v>30</v>
       </c>
       <c r="K26">
-        <v>1584.5623000000001</v>
+        <v>17722.396000000001</v>
       </c>
       <c r="L26">
         <v>58.906647</v>
@@ -2611,7 +2611,7 @@
         <v>51</v>
       </c>
       <c r="K27">
-        <v>1609.2815000000001</v>
+        <v>28764.782999999999</v>
       </c>
       <c r="L27">
         <v>100.1413</v>
@@ -2652,7 +2652,7 @@
         <v>196</v>
       </c>
       <c r="K28">
-        <v>1584.2260000000001</v>
+        <v>120153.89</v>
       </c>
       <c r="L28">
         <v>384.85674999999998</v>
@@ -2693,7 +2693,7 @@
         <v>46</v>
       </c>
       <c r="K29">
-        <v>1661.1687999999999</v>
+        <v>26889.47</v>
       </c>
       <c r="L29">
         <v>90.323524000000006</v>
@@ -2734,7 +2734,7 @@
         <v>73</v>
       </c>
       <c r="K30">
-        <v>1663.7739999999999</v>
+        <v>43730.133000000002</v>
       </c>
       <c r="L30">
         <v>143.33950999999999</v>
@@ -2775,7 +2775,7 @@
         <v>115</v>
       </c>
       <c r="K31">
-        <v>1584.9971</v>
+        <v>64794.336000000003</v>
       </c>
       <c r="L31">
         <v>225.80879999999999</v>
@@ -2816,7 +2816,7 @@
         <v>822</v>
       </c>
       <c r="K32">
-        <v>1576.8373999999999</v>
+        <v>504351</v>
       </c>
       <c r="L32">
         <v>1614.0420999999999</v>
@@ -2857,7 +2857,7 @@
         <v>104</v>
       </c>
       <c r="K33">
-        <v>1665.7626</v>
+        <v>63327.042999999998</v>
       </c>
       <c r="L33">
         <v>204.2097</v>
@@ -2898,7 +2898,7 @@
         <v>212</v>
       </c>
       <c r="K34">
-        <v>1570.9668999999999</v>
+        <v>122112.23</v>
       </c>
       <c r="L34">
         <v>416.27361999999999</v>
@@ -2939,7 +2939,7 @@
         <v>58</v>
       </c>
       <c r="K35">
-        <v>1584.8844999999999</v>
+        <v>35462.75</v>
       </c>
       <c r="L35">
         <v>113.886185</v>
@@ -2980,7 +2980,7 @@
         <v>144</v>
       </c>
       <c r="K36">
-        <v>1698.2602999999999</v>
+        <v>82257.33</v>
       </c>
       <c r="L36">
         <v>282.75189999999998</v>
@@ -3021,7 +3021,7 @@
         <v>59</v>
       </c>
       <c r="K37">
-        <v>1630.7167999999999</v>
+        <v>29164.728999999999</v>
       </c>
       <c r="L37">
         <v>115.84974</v>
@@ -3062,7 +3062,7 @@
         <v>858</v>
       </c>
       <c r="K38">
-        <v>1588.1403</v>
+        <v>525867.4</v>
       </c>
       <c r="L38">
         <v>1684.7301</v>
@@ -3103,7 +3103,7 @@
         <v>159</v>
       </c>
       <c r="K39">
-        <v>1659.2025000000001</v>
+        <v>88922.61</v>
       </c>
       <c r="L39">
         <v>312.20522999999997</v>
@@ -3144,7 +3144,7 @@
         <v>158</v>
       </c>
       <c r="K40">
-        <v>1492.2592999999999</v>
+        <v>85687.59</v>
       </c>
       <c r="L40">
         <v>310.24167</v>
@@ -3185,7 +3185,7 @@
         <v>711</v>
       </c>
       <c r="K41">
-        <v>1597.864</v>
+        <v>375119.9</v>
       </c>
       <c r="L41">
         <v>1396.0875000000001</v>
@@ -3226,7 +3226,7 @@
         <v>54</v>
       </c>
       <c r="K42">
-        <v>1570.1763000000001</v>
+        <v>32381.828000000001</v>
       </c>
       <c r="L42">
         <v>106.03196</v>
@@ -3267,7 +3267,7 @@
         <v>784</v>
       </c>
       <c r="K43">
-        <v>1577.2775999999999</v>
+        <v>479701.84</v>
       </c>
       <c r="L43">
         <v>1539.4269999999999</v>
@@ -3308,7 +3308,7 @@
         <v>33</v>
       </c>
       <c r="K44">
-        <v>1607.3677</v>
+        <v>18154.312999999998</v>
       </c>
       <c r="L44">
         <v>64.797309999999996</v>
@@ -3349,7 +3349,7 @@
         <v>64</v>
       </c>
       <c r="K45">
-        <v>1595.9052999999999</v>
+        <v>36187.152000000002</v>
       </c>
       <c r="L45">
         <v>125.66750999999999</v>
@@ -3390,7 +3390,7 @@
         <v>187</v>
       </c>
       <c r="K46">
-        <v>1646.7550000000001</v>
+        <v>109277.71</v>
       </c>
       <c r="L46">
         <v>367.18475000000001</v>
@@ -3431,7 +3431,7 @@
         <v>159</v>
       </c>
       <c r="K47">
-        <v>1492.0681999999999</v>
+        <v>90219.6</v>
       </c>
       <c r="L47">
         <v>312.20522999999997</v>
@@ -3472,7 +3472,7 @@
         <v>62</v>
       </c>
       <c r="K48">
-        <v>1606.7845</v>
+        <v>38230.535000000003</v>
       </c>
       <c r="L48">
         <v>121.74039999999999</v>
@@ -3513,7 +3513,7 @@
         <v>515</v>
       </c>
       <c r="K49">
-        <v>1613.1375</v>
+        <v>313997.03000000003</v>
       </c>
       <c r="L49">
         <v>1011.2308</v>
@@ -3554,7 +3554,7 @@
         <v>75</v>
       </c>
       <c r="K50">
-        <v>1562.2782</v>
+        <v>44513.57</v>
       </c>
       <c r="L50">
         <v>147.26661999999999</v>
@@ -3595,7 +3595,7 @@
         <v>62</v>
       </c>
       <c r="K51">
-        <v>1290.4568999999999</v>
+        <v>26148.68</v>
       </c>
       <c r="L51">
         <v>121.74039999999999</v>
@@ -3636,7 +3636,7 @@
         <v>27</v>
       </c>
       <c r="K52">
-        <v>1530.816</v>
+        <v>13010.584999999999</v>
       </c>
       <c r="L52">
         <v>53.015979999999999</v>
@@ -3677,7 +3677,7 @@
         <v>77</v>
       </c>
       <c r="K53">
-        <v>1658.4258</v>
+        <v>49924.18</v>
       </c>
       <c r="L53">
         <v>151.19372999999999</v>
@@ -3718,7 +3718,7 @@
         <v>73</v>
       </c>
       <c r="K54">
-        <v>1654.8463999999999</v>
+        <v>40183.105000000003</v>
       </c>
       <c r="L54">
         <v>143.33950999999999</v>
@@ -3759,7 +3759,7 @@
         <v>3527</v>
       </c>
       <c r="K55">
-        <v>1575.4855</v>
+        <v>2079884.8</v>
       </c>
       <c r="L55">
         <v>6925.4579999999996</v>
@@ -3800,7 +3800,7 @@
         <v>38</v>
       </c>
       <c r="K56">
-        <v>1644.3524</v>
+        <v>20493.228999999999</v>
       </c>
       <c r="L56">
         <v>74.615080000000006</v>
@@ -3841,7 +3841,7 @@
         <v>156</v>
       </c>
       <c r="K57">
-        <v>1489.527</v>
+        <v>86055.78</v>
       </c>
       <c r="L57">
         <v>306.31454000000002</v>
@@ -3882,7 +3882,7 @@
         <v>685</v>
       </c>
       <c r="K58">
-        <v>1573.2428</v>
+        <v>362068.38</v>
       </c>
       <c r="L58">
         <v>1345.0350000000001</v>
@@ -3923,7 +3923,7 @@
         <v>9</v>
       </c>
       <c r="K59">
-        <v>1683.2267999999999</v>
+        <v>5291.6934000000001</v>
       </c>
       <c r="L59">
         <v>17.671993000000001</v>
@@ -3964,7 +3964,7 @@
         <v>91</v>
       </c>
       <c r="K60">
-        <v>1548.1699000000001</v>
+        <v>53592.495999999999</v>
       </c>
       <c r="L60">
         <v>178.68349000000001</v>
@@ -4005,7 +4005,7 @@
         <v>41</v>
       </c>
       <c r="K61">
-        <v>1385.9257</v>
+        <v>21184.440999999999</v>
       </c>
       <c r="L61">
         <v>80.505750000000006</v>
@@ -4046,7 +4046,7 @@
         <v>502</v>
       </c>
       <c r="K62">
-        <v>1609.6538</v>
+        <v>316975.15999999997</v>
       </c>
       <c r="L62">
         <v>985.70450000000005</v>

</xml_diff>

<commit_message>
Finished adding data for numPanels, yearlyEnergy, and solarArea columns
</commit_message>
<xml_diff>
--- a/SolarApiLocations.xlsx
+++ b/SolarApiLocations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d353e6827118956a/addressToDistance/addressToExcel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/jelliott48_gatech_edu/Documents/Documents/Fall24/ECE 3600/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="507" documentId="11_217FF8C2F712DE19CC611F02D8539FE741A2C757" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CC09D75-EAD3-4B4E-A09F-8C6B254AE905}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="11_217FF8C2F712DE19CC611F02D8539FE741A2C757" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69192241-75B3-F24B-8CBC-6A360017B62B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="369">
   <si>
     <t>Name</t>
   </si>
@@ -806,9 +806,6 @@
     <t>581 Metropolitan Pkwy SW, Atlanta, GA 30310</t>
   </si>
   <si>
-    <t>Slutty Vegan</t>
-  </si>
-  <si>
     <t>476 Edgewood Ave SE, Atlanta, GA 30312</t>
   </si>
   <si>
@@ -869,9 +866,6 @@
     <t>473 Broad St, Augusta, GA 30901</t>
   </si>
   <si>
-    <t>Sublime Doughnuts</t>
-  </si>
-  <si>
     <t>535 10th St NW, Atlanta, GA 30318</t>
   </si>
   <si>
@@ -1028,15 +1022,9 @@
     <t>12353 Veterans Memorial Highway, 6668 W Broad St, Douglasville, GA 30134</t>
   </si>
   <si>
-    <t>Toast on Lenox</t>
-  </si>
-  <si>
     <t>349 14th St NW, Atlanta, GA 30318</t>
   </si>
   <si>
-    <t>Toast On Lenox</t>
-  </si>
-  <si>
     <t>2770 Lenox Rd NE, Atlanta, GA 30324</t>
   </si>
   <si>
@@ -1137,6 +1125,24 @@
   </si>
   <si>
     <t>Google Maps</t>
+  </si>
+  <si>
+    <t>Slutty Vegan McDonough</t>
+  </si>
+  <si>
+    <t>Slutty Vegan Edgewood</t>
+  </si>
+  <si>
+    <t>Sublime Doughnuts 10th Street</t>
+  </si>
+  <si>
+    <t>Sublime Doughnuts Briarcliff</t>
+  </si>
+  <si>
+    <t>Toast on Lenox 14th Street</t>
+  </si>
+  <si>
+    <t>Toast On Lenox Lenox</t>
   </si>
 </sst>
 </file>
@@ -1526,35 +1532,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="103" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63:L182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.69921875" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="9.09765625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
     <col min="7" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="20.5" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
     <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1583,16 +1589,16 @@
         <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="K2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="L2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>1060.3196</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1674,7 +1680,7 @@
         <v>486.96159999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>2034.2428</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>123.70396</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>323.98653999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1838,7 +1844,7 @@
         <v>54.979537999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>76.578636000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1920,7 +1926,7 @@
         <v>113.886185</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>795.23974999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>1260.6022</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>726.51530000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2084,7 +2090,7 @@
         <v>8894.9030000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>129.7988</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>49.08887</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>867.89124000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>111.92263</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>600.84780000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -2330,7 +2336,7 @@
         <v>100.1413</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>956.25120000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>2493.7145999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>341.65854000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>516.41489999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>64.797309999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2576,7 +2582,7 @@
         <v>58.906647</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>100.1413</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>384.85674999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>90.323524000000006</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2740,7 +2746,7 @@
         <v>143.33950999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>225.80879999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>1614.0420999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>204.2097</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>416.27361999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>113.886185</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>282.75189999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -3027,7 +3033,7 @@
         <v>115.84974</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>1684.7301</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -3109,7 +3115,7 @@
         <v>312.20522999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -3150,7 +3156,7 @@
         <v>310.24167</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>1396.0875000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -3232,7 +3238,7 @@
         <v>106.03196</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -3273,7 +3279,7 @@
         <v>1539.4269999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>64.797309999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -3355,7 +3361,7 @@
         <v>125.66750999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>367.18475000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -3437,7 +3443,7 @@
         <v>312.20522999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -3478,7 +3484,7 @@
         <v>121.74039999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -3519,7 +3525,7 @@
         <v>1011.2308</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -3560,7 +3566,7 @@
         <v>147.26661999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -3601,7 +3607,7 @@
         <v>121.74039999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -3642,7 +3648,7 @@
         <v>53.015979999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -3683,7 +3689,7 @@
         <v>151.19372999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>143.33950999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>6925.4579999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -3806,7 +3812,7 @@
         <v>74.615080000000006</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -3847,7 +3853,7 @@
         <v>306.31454000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>1345.0350000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -3929,7 +3935,7 @@
         <v>17.671993000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -3970,7 +3976,7 @@
         <v>178.68349000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -4011,7 +4017,7 @@
         <v>80.505750000000006</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -4052,7 +4058,7 @@
         <v>985.70450000000005</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>127</v>
       </c>
@@ -4083,8 +4089,17 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J63">
+        <v>52</v>
+      </c>
+      <c r="K63">
+        <v>18737.393</v>
+      </c>
+      <c r="L63">
+        <v>102.10485</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>129</v>
       </c>
@@ -4115,8 +4130,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J64">
+        <v>80</v>
+      </c>
+      <c r="K64">
+        <v>49429.008000000002</v>
+      </c>
+      <c r="L64">
+        <v>157.08438000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>131</v>
       </c>
@@ -4147,8 +4171,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J65">
+        <v>114</v>
+      </c>
+      <c r="K65">
+        <v>69919.48</v>
+      </c>
+      <c r="L65">
+        <v>223.84526</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -4179,8 +4212,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66">
+        <v>81</v>
+      </c>
+      <c r="K66">
+        <v>48009.402000000002</v>
+      </c>
+      <c r="L66">
+        <v>159.04794000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -4211,8 +4253,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J67">
+        <v>110</v>
+      </c>
+      <c r="K67">
+        <v>54934.074000000001</v>
+      </c>
+      <c r="L67">
+        <v>215.99102999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -4243,8 +4294,17 @@
         <f t="shared" ref="I68:I131" si="5">IF(OR(G68 &gt; 0.1, H68 &gt; 0.1), "1", "0")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J68">
+        <v>71</v>
+      </c>
+      <c r="K68">
+        <v>33310.959999999999</v>
+      </c>
+      <c r="L68">
+        <v>139.41239999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>139</v>
       </c>
@@ -4275,8 +4335,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J69">
+        <v>142</v>
+      </c>
+      <c r="K69">
+        <v>82909.125</v>
+      </c>
+      <c r="L69">
+        <v>278.82479999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>141</v>
       </c>
@@ -4307,8 +4376,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J70">
+        <v>502</v>
+      </c>
+      <c r="K70">
+        <v>316975.15999999997</v>
+      </c>
+      <c r="L70">
+        <v>985.70450000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -4339,8 +4417,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71">
+        <v>597</v>
+      </c>
+      <c r="K71">
+        <v>344774.16</v>
+      </c>
+      <c r="L71">
+        <v>1172.2422999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>145</v>
       </c>
@@ -4371,8 +4458,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J72">
+        <v>97</v>
+      </c>
+      <c r="K72">
+        <v>49309.934000000001</v>
+      </c>
+      <c r="L72">
+        <v>190.46483000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>147</v>
       </c>
@@ -4403,8 +4499,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J73">
+        <v>310</v>
+      </c>
+      <c r="K73">
+        <v>190421.75</v>
+      </c>
+      <c r="L73">
+        <v>608.702</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -4435,8 +4540,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J74">
+        <v>26</v>
+      </c>
+      <c r="K74">
+        <v>14267.599</v>
+      </c>
+      <c r="L74">
+        <v>51.052424999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>151</v>
       </c>
@@ -4467,8 +4581,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J75">
+        <v>34</v>
+      </c>
+      <c r="K75">
+        <v>20253.280999999999</v>
+      </c>
+      <c r="L75">
+        <v>66.760863999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>153</v>
       </c>
@@ -4499,8 +4622,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J76">
+        <v>187</v>
+      </c>
+      <c r="K76">
+        <v>104780.26</v>
+      </c>
+      <c r="L76">
+        <v>367.18475000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -4531,8 +4663,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J77">
+        <v>118</v>
+      </c>
+      <c r="K77">
+        <v>60355.207000000002</v>
+      </c>
+      <c r="L77">
+        <v>231.69947999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -4563,8 +4704,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J78">
+        <v>53</v>
+      </c>
+      <c r="K78">
+        <v>32035.115000000002</v>
+      </c>
+      <c r="L78">
+        <v>104.068405</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -4595,8 +4745,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J79">
+        <v>275</v>
+      </c>
+      <c r="K79">
+        <v>166204.03</v>
+      </c>
+      <c r="L79">
+        <v>539.97760000000005</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>161</v>
       </c>
@@ -4627,8 +4786,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J80">
+        <v>42</v>
+      </c>
+      <c r="K80">
+        <v>25216.03</v>
+      </c>
+      <c r="L80">
+        <v>82.469309999999993</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -4659,8 +4827,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J81">
+        <v>156</v>
+      </c>
+      <c r="K81">
+        <v>86055.78</v>
+      </c>
+      <c r="L81">
+        <v>306.31454000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>164</v>
       </c>
@@ -4691,8 +4868,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J82">
+        <v>177</v>
+      </c>
+      <c r="K82">
+        <v>103876.41</v>
+      </c>
+      <c r="L82">
+        <v>347.54921999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>166</v>
       </c>
@@ -4723,8 +4909,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J83">
+        <v>47</v>
+      </c>
+      <c r="K83">
+        <v>26713.99</v>
+      </c>
+      <c r="L83">
+        <v>92.287080000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>168</v>
       </c>
@@ -4755,8 +4950,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J84">
+        <v>1614</v>
+      </c>
+      <c r="K84">
+        <v>899587.94</v>
+      </c>
+      <c r="L84">
+        <v>3169.1774999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>170</v>
       </c>
@@ -4787,8 +4991,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J85">
+        <v>31</v>
+      </c>
+      <c r="K85">
+        <v>14615.36</v>
+      </c>
+      <c r="L85">
+        <v>60.870199999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>172</v>
       </c>
@@ -4819,8 +5032,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J86">
+        <v>54</v>
+      </c>
+      <c r="K86">
+        <v>32381.828000000001</v>
+      </c>
+      <c r="L86">
+        <v>106.03196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -4851,8 +5073,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J87">
+        <v>31</v>
+      </c>
+      <c r="K87">
+        <v>14615.36</v>
+      </c>
+      <c r="L87">
+        <v>60.870199999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>176</v>
       </c>
@@ -4883,8 +5114,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J88">
+        <v>701</v>
+      </c>
+      <c r="K88">
+        <v>379896.97</v>
+      </c>
+      <c r="L88">
+        <v>1376.4519</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -4915,8 +5155,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J89">
+        <v>163</v>
+      </c>
+      <c r="K89">
+        <v>96094.69</v>
+      </c>
+      <c r="L89">
+        <v>320.05945000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -4947,8 +5196,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J90">
+        <v>226</v>
+      </c>
+      <c r="K90">
+        <v>131312.47</v>
+      </c>
+      <c r="L90">
+        <v>443.76339999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>182</v>
       </c>
@@ -4979,8 +5237,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J91">
+        <v>34</v>
+      </c>
+      <c r="K91">
+        <v>12983.191999999999</v>
+      </c>
+      <c r="L91">
+        <v>66.760863999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>184</v>
       </c>
@@ -5011,8 +5278,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J92">
+        <v>86</v>
+      </c>
+      <c r="K92">
+        <v>47995.023000000001</v>
+      </c>
+      <c r="L92">
+        <v>168.86572000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>186</v>
       </c>
@@ -5043,8 +5319,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J93">
+        <v>144</v>
+      </c>
+      <c r="K93">
+        <v>86613.85</v>
+      </c>
+      <c r="L93">
+        <v>282.75189999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>188</v>
       </c>
@@ -5075,8 +5360,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J94">
+        <v>242</v>
+      </c>
+      <c r="K94">
+        <v>149661</v>
+      </c>
+      <c r="L94">
+        <v>475.18027000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>190</v>
       </c>
@@ -5107,8 +5401,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J95">
+        <v>45</v>
+      </c>
+      <c r="K95">
+        <v>22448.728999999999</v>
+      </c>
+      <c r="L95">
+        <v>88.359970000000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>192</v>
       </c>
@@ -5139,8 +5442,17 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J96">
+        <v>131</v>
+      </c>
+      <c r="K96">
+        <v>74785.554999999993</v>
+      </c>
+      <c r="L96">
+        <v>257.22568000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>194</v>
       </c>
@@ -5171,8 +5483,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J97">
+        <v>444</v>
+      </c>
+      <c r="K97">
+        <v>217293</v>
+      </c>
+      <c r="L97">
+        <v>871.81835999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>196</v>
       </c>
@@ -5203,8 +5524,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J98">
+        <v>69</v>
+      </c>
+      <c r="K98">
+        <v>32885.233999999997</v>
+      </c>
+      <c r="L98">
+        <v>135.48528999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>198</v>
       </c>
@@ -5235,8 +5565,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J99">
+        <v>159</v>
+      </c>
+      <c r="K99">
+        <v>97232.09</v>
+      </c>
+      <c r="L99">
+        <v>312.20522999999997</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>200</v>
       </c>
@@ -5267,8 +5606,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J100">
+        <v>51</v>
+      </c>
+      <c r="K100">
+        <v>27218.678</v>
+      </c>
+      <c r="L100">
+        <v>100.1413</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>202</v>
       </c>
@@ -5299,8 +5647,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J101">
+        <v>62</v>
+      </c>
+      <c r="K101">
+        <v>34683.546999999999</v>
+      </c>
+      <c r="L101">
+        <v>121.74039999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>204</v>
       </c>
@@ -5331,8 +5688,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J102">
+        <v>83</v>
+      </c>
+      <c r="K102">
+        <v>50394.836000000003</v>
+      </c>
+      <c r="L102">
+        <v>162.97505000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>206</v>
       </c>
@@ -5363,8 +5729,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J103">
+        <v>57</v>
+      </c>
+      <c r="K103">
+        <v>30222.206999999999</v>
+      </c>
+      <c r="L103">
+        <v>111.92263</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>208</v>
       </c>
@@ -5395,8 +5770,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J104">
+        <v>91</v>
+      </c>
+      <c r="K104">
+        <v>51122.745999999999</v>
+      </c>
+      <c r="L104">
+        <v>178.68349000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>210</v>
       </c>
@@ -5427,8 +5811,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J105">
+        <v>644</v>
+      </c>
+      <c r="K105">
+        <v>365734.03</v>
+      </c>
+      <c r="L105">
+        <v>1264.5292999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>212</v>
       </c>
@@ -5459,8 +5852,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J106">
+        <v>405</v>
+      </c>
+      <c r="K106">
+        <v>206903.03</v>
+      </c>
+      <c r="L106">
+        <v>795.23974999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>213</v>
       </c>
@@ -5491,8 +5893,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J107">
+        <v>90</v>
+      </c>
+      <c r="K107">
+        <v>54021.203000000001</v>
+      </c>
+      <c r="L107">
+        <v>176.71994000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>215</v>
       </c>
@@ -5523,8 +5934,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J108">
+        <v>39</v>
+      </c>
+      <c r="K108">
+        <v>21568.734</v>
+      </c>
+      <c r="L108">
+        <v>76.578636000000003</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>217</v>
       </c>
@@ -5555,8 +5975,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J109">
+        <v>77</v>
+      </c>
+      <c r="K109">
+        <v>43016.51</v>
+      </c>
+      <c r="L109">
+        <v>151.19372999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>219</v>
       </c>
@@ -5587,8 +6016,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J110">
+        <v>302</v>
+      </c>
+      <c r="K110">
+        <v>185321.34</v>
+      </c>
+      <c r="L110">
+        <v>592.99360000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>221</v>
       </c>
@@ -5619,8 +6057,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J111">
+        <v>178</v>
+      </c>
+      <c r="K111">
+        <v>109520.19</v>
+      </c>
+      <c r="L111">
+        <v>349.51276000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>223</v>
       </c>
@@ -5651,8 +6098,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J112">
+        <v>59</v>
+      </c>
+      <c r="K112">
+        <v>27434.502</v>
+      </c>
+      <c r="L112">
+        <v>115.84974</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>225</v>
       </c>
@@ -5683,8 +6139,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J113">
+        <v>97</v>
+      </c>
+      <c r="K113">
+        <v>57024.008000000002</v>
+      </c>
+      <c r="L113">
+        <v>190.46483000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>227</v>
       </c>
@@ -5715,8 +6180,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J114">
+        <v>276</v>
+      </c>
+      <c r="K114">
+        <v>172367.83</v>
+      </c>
+      <c r="L114">
+        <v>541.94115999999997</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>229</v>
       </c>
@@ -5747,8 +6221,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J115">
+        <v>85</v>
+      </c>
+      <c r="K115">
+        <v>51610.805</v>
+      </c>
+      <c r="L115">
+        <v>166.90216000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>231</v>
       </c>
@@ -5779,8 +6262,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J116">
+        <v>21</v>
+      </c>
+      <c r="K116">
+        <v>10737.646000000001</v>
+      </c>
+      <c r="L116">
+        <v>41.234653000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>233</v>
       </c>
@@ -5811,8 +6303,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J117">
+        <v>27</v>
+      </c>
+      <c r="K117">
+        <v>10997.812</v>
+      </c>
+      <c r="L117">
+        <v>53.015979999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>235</v>
       </c>
@@ -5843,8 +6344,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J118">
+        <v>105</v>
+      </c>
+      <c r="K118">
+        <v>48861.226999999999</v>
+      </c>
+      <c r="L118">
+        <v>206.17326</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>237</v>
       </c>
@@ -5875,8 +6385,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J119">
+        <v>44</v>
+      </c>
+      <c r="K119">
+        <v>18556.822</v>
+      </c>
+      <c r="L119">
+        <v>86.396416000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>239</v>
       </c>
@@ -5907,8 +6426,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J120">
+        <v>59</v>
+      </c>
+      <c r="K120">
+        <v>33454.495999999999</v>
+      </c>
+      <c r="L120">
+        <v>115.84974</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>241</v>
       </c>
@@ -5939,8 +6467,17 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J121">
+        <v>88</v>
+      </c>
+      <c r="K121">
+        <v>48923.09</v>
+      </c>
+      <c r="L121">
+        <v>172.79283000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>243</v>
       </c>
@@ -5971,8 +6508,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J122">
+        <v>73</v>
+      </c>
+      <c r="K122">
+        <v>43358.315999999999</v>
+      </c>
+      <c r="L122">
+        <v>143.33950999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>245</v>
       </c>
@@ -6003,8 +6549,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J123">
+        <v>143</v>
+      </c>
+      <c r="K123">
+        <v>71239.039999999994</v>
+      </c>
+      <c r="L123">
+        <v>280.78832999999997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>247</v>
       </c>
@@ -6035,8 +6590,17 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J124">
+        <v>104</v>
+      </c>
+      <c r="K124">
+        <v>61771.453000000001</v>
+      </c>
+      <c r="L124">
+        <v>204.2097</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>249</v>
       </c>
@@ -6067,8 +6631,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J125">
+        <v>42</v>
+      </c>
+      <c r="K125">
+        <v>24369.455000000002</v>
+      </c>
+      <c r="L125">
+        <v>82.469309999999993</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>251</v>
       </c>
@@ -6099,8 +6672,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J126">
+        <v>40</v>
+      </c>
+      <c r="K126">
+        <v>18206.252</v>
+      </c>
+      <c r="L126">
+        <v>78.542190000000005</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>253</v>
       </c>
@@ -6131,8 +6713,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J127">
+        <v>57</v>
+      </c>
+      <c r="K127">
+        <v>30222.206999999999</v>
+      </c>
+      <c r="L127">
+        <v>111.92263</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -6163,13 +6754,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J128">
+        <v>75</v>
+      </c>
+      <c r="K128">
+        <v>41834.188000000002</v>
+      </c>
+      <c r="L128">
+        <v>147.26661999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>364</v>
+      </c>
+      <c r="B129" t="s">
         <v>256</v>
-      </c>
-      <c r="B129" t="s">
-        <v>257</v>
       </c>
       <c r="C129">
         <v>33.754378000000003</v>
@@ -6195,13 +6795,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J129">
+        <v>138</v>
+      </c>
+      <c r="K129">
+        <v>81442.304999999993</v>
+      </c>
+      <c r="L129">
+        <v>270.97057999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>256</v>
+        <v>363</v>
       </c>
       <c r="B130" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C130">
         <v>33.525095999999998</v>
@@ -6227,13 +6836,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J130">
+        <v>348</v>
+      </c>
+      <c r="K130">
+        <v>196594.86</v>
+      </c>
+      <c r="L130">
+        <v>683.31709999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>258</v>
+      </c>
+      <c r="B131" t="s">
         <v>259</v>
-      </c>
-      <c r="B131" t="s">
-        <v>260</v>
       </c>
       <c r="C131">
         <v>34.0066214</v>
@@ -6259,13 +6877,22 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J131">
+        <v>66</v>
+      </c>
+      <c r="K131">
+        <v>40822.065999999999</v>
+      </c>
+      <c r="L131">
+        <v>129.59461999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>260</v>
+      </c>
+      <c r="B132" t="s">
         <v>261</v>
-      </c>
-      <c r="B132" t="s">
-        <v>262</v>
       </c>
       <c r="C132">
         <v>33.743516</v>
@@ -6291,13 +6918,22 @@
         <f t="shared" ref="I132:I181" si="8">IF(OR(G132 &gt; 0.1, H132 &gt; 0.1), "1", "0")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J132">
+        <v>42</v>
+      </c>
+      <c r="K132">
+        <v>21377.643</v>
+      </c>
+      <c r="L132">
+        <v>82.469309999999993</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>262</v>
+      </c>
+      <c r="B133" t="s">
         <v>263</v>
-      </c>
-      <c r="B133" t="s">
-        <v>264</v>
       </c>
       <c r="C133">
         <v>33.772205399999997</v>
@@ -6323,13 +6959,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J133">
+        <v>136</v>
+      </c>
+      <c r="K133">
+        <v>81245.7</v>
+      </c>
+      <c r="L133">
+        <v>267.04345999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>264</v>
+      </c>
+      <c r="B134" t="s">
         <v>265</v>
-      </c>
-      <c r="B134" t="s">
-        <v>266</v>
       </c>
       <c r="C134">
         <v>33.738167799999999</v>
@@ -6355,13 +7000,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J134">
+        <v>66</v>
+      </c>
+      <c r="K134">
+        <v>41587.042999999998</v>
+      </c>
+      <c r="L134">
+        <v>129.59461999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>266</v>
+      </c>
+      <c r="B135" t="s">
         <v>267</v>
-      </c>
-      <c r="B135" t="s">
-        <v>268</v>
       </c>
       <c r="C135">
         <v>33.876629000000001</v>
@@ -6387,13 +7041,22 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J135">
+        <v>732</v>
+      </c>
+      <c r="K135">
+        <v>446733.22</v>
+      </c>
+      <c r="L135">
+        <v>1437.3221000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>268</v>
+      </c>
+      <c r="B136" t="s">
         <v>269</v>
-      </c>
-      <c r="B136" t="s">
-        <v>270</v>
       </c>
       <c r="C136">
         <v>33.886471999999998</v>
@@ -6419,13 +7082,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J136">
+        <v>1027</v>
+      </c>
+      <c r="K136">
+        <v>628114.80000000005</v>
+      </c>
+      <c r="L136">
+        <v>2016.5708</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>270</v>
+      </c>
+      <c r="B137" t="s">
         <v>271</v>
-      </c>
-      <c r="B137" t="s">
-        <v>272</v>
       </c>
       <c r="C137">
         <v>33.736809000000001</v>
@@ -6451,13 +7123,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J137">
+        <v>48</v>
+      </c>
+      <c r="K137">
+        <v>28080.412</v>
+      </c>
+      <c r="L137">
+        <v>94.250630000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>272</v>
+      </c>
+      <c r="B138" t="s">
         <v>273</v>
-      </c>
-      <c r="B138" t="s">
-        <v>274</v>
       </c>
       <c r="C138">
         <v>33.747542000000003</v>
@@ -6483,13 +7164,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J138">
+        <v>24</v>
+      </c>
+      <c r="K138">
+        <v>13332.897999999999</v>
+      </c>
+      <c r="L138">
+        <v>47.125317000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>274</v>
+      </c>
+      <c r="B139" t="s">
         <v>275</v>
-      </c>
-      <c r="B139" t="s">
-        <v>276</v>
       </c>
       <c r="C139">
         <v>33.472682599999999</v>
@@ -6515,13 +7205,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J139">
+        <v>147</v>
+      </c>
+      <c r="K139">
+        <v>84517.41</v>
+      </c>
+      <c r="L139">
+        <v>288.64258000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>277</v>
+        <v>365</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C140">
         <v>33.781856400000002</v>
@@ -6547,13 +7246,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J140">
+        <v>584</v>
+      </c>
+      <c r="K140">
+        <v>330379.78000000003</v>
+      </c>
+      <c r="L140">
+        <v>1146.7161000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>366</v>
+      </c>
+      <c r="B141" t="s">
         <v>277</v>
-      </c>
-      <c r="B141" t="s">
-        <v>279</v>
       </c>
       <c r="C141">
         <v>33.8284533</v>
@@ -6579,13 +7287,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J141">
+        <v>597</v>
+      </c>
+      <c r="K141">
+        <v>344514.25</v>
+      </c>
+      <c r="L141">
+        <v>1172.2422999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B142" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C142">
         <v>33.531801000000002</v>
@@ -6611,13 +7328,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J142">
+        <v>50</v>
+      </c>
+      <c r="K142">
+        <v>31221.759999999998</v>
+      </c>
+      <c r="L142">
+        <v>98.17774</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B143" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C143">
         <v>33.583321099999999</v>
@@ -6643,13 +7369,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J143">
+        <v>540</v>
+      </c>
+      <c r="K143">
+        <v>333510.13</v>
+      </c>
+      <c r="L143">
+        <v>1060.3196</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B144" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C144">
         <v>33.750441799999997</v>
@@ -6675,13 +7410,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J144">
+        <v>39</v>
+      </c>
+      <c r="K144">
+        <v>17985.006000000001</v>
+      </c>
+      <c r="L144">
+        <v>76.578636000000003</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B145" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C145">
         <v>33.738387400000001</v>
@@ -6707,13 +7451,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J145">
+        <v>97</v>
+      </c>
+      <c r="K145">
+        <v>57024.008000000002</v>
+      </c>
+      <c r="L145">
+        <v>190.46483000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B146" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C146">
         <v>33.773077000000001</v>
@@ -6739,13 +7492,22 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J146">
+        <v>549</v>
+      </c>
+      <c r="K146">
+        <v>324342.34000000003</v>
+      </c>
+      <c r="L146">
+        <v>1077.9916000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B147" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C147">
         <v>33.740399099999998</v>
@@ -6771,13 +7533,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J147">
+        <v>7</v>
+      </c>
+      <c r="K147">
+        <v>4212.2744000000002</v>
+      </c>
+      <c r="L147">
+        <v>13.7448845</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B148" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C148">
         <v>33.800226000000002</v>
@@ -6803,13 +7574,22 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J148">
+        <v>487</v>
+      </c>
+      <c r="K148">
+        <v>296738.40000000002</v>
+      </c>
+      <c r="L148">
+        <v>956.25120000000004</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B149" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C149">
         <v>33.722276600000001</v>
@@ -6835,13 +7615,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J149">
+        <v>61</v>
+      </c>
+      <c r="K149">
+        <v>36085.055</v>
+      </c>
+      <c r="L149">
+        <v>119.77685</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B150" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C150">
         <v>33.740657200000001</v>
@@ -6867,13 +7656,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J150">
+        <v>30</v>
+      </c>
+      <c r="K150">
+        <v>16912.851999999999</v>
+      </c>
+      <c r="L150">
+        <v>58.906647</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B151" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C151">
         <v>33.945991999999997</v>
@@ -6899,13 +7697,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J151">
+        <v>24</v>
+      </c>
+      <c r="K151">
+        <v>13748.722</v>
+      </c>
+      <c r="L151">
+        <v>47.125317000000003</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B152" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C152">
         <v>33.754531</v>
@@ -6931,13 +7738,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J152">
+        <v>76</v>
+      </c>
+      <c r="K152">
+        <v>43858.065999999999</v>
+      </c>
+      <c r="L152">
+        <v>149.23016000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B153" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C153">
         <v>33.663263899999997</v>
@@ -6963,13 +7779,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J153">
+        <v>94</v>
+      </c>
+      <c r="K153">
+        <v>55848.563000000002</v>
+      </c>
+      <c r="L153">
+        <v>184.57416000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B154" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C154">
         <v>33.781421299999998</v>
@@ -6995,13 +7820,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J154">
+        <v>325</v>
+      </c>
+      <c r="K154">
+        <v>155863.78</v>
+      </c>
+      <c r="L154">
+        <v>638.15533000000005</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B155" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C155">
         <v>33.650859400000002</v>
@@ -7027,13 +7861,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J155">
+        <v>135</v>
+      </c>
+      <c r="K155">
+        <v>74776.679999999993</v>
+      </c>
+      <c r="L155">
+        <v>265.07990000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B156" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C156">
         <v>33.758375299999997</v>
@@ -7059,13 +7902,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J156">
+        <v>201</v>
+      </c>
+      <c r="K156">
+        <v>96264.54</v>
+      </c>
+      <c r="L156">
+        <v>394.67453</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B157" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C157">
         <v>33.7859281</v>
@@ -7091,13 +7943,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J157">
+        <v>132</v>
+      </c>
+      <c r="K157">
+        <v>76885.64</v>
+      </c>
+      <c r="L157">
+        <v>259.18923999999998</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B158" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C158">
         <v>33.810287700000003</v>
@@ -7123,13 +7984,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J158">
+        <v>1129</v>
+      </c>
+      <c r="K158">
+        <v>661070.80000000005</v>
+      </c>
+      <c r="L158">
+        <v>2216.8535000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B159" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C159">
         <v>33.809074000000003</v>
@@ -7155,13 +8025,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J159">
+        <v>1384</v>
+      </c>
+      <c r="K159">
+        <v>729206.2</v>
+      </c>
+      <c r="L159">
+        <v>2717.5598</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B160" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C160">
         <v>33.755504299999998</v>
@@ -7187,13 +8066,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J160">
+        <v>354</v>
+      </c>
+      <c r="K160">
+        <v>208539.61</v>
+      </c>
+      <c r="L160">
+        <v>695.09844999999996</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B161" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C161">
         <v>33.602426999999999</v>
@@ -7219,13 +8107,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J161">
+        <v>530</v>
+      </c>
+      <c r="K161">
+        <v>323442.2</v>
+      </c>
+      <c r="L161">
+        <v>1040.6840999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B162" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C162">
         <v>33.484462000000001</v>
@@ -7251,13 +8148,22 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J162">
+        <v>412</v>
+      </c>
+      <c r="K162">
+        <v>253523.45</v>
+      </c>
+      <c r="L162">
+        <v>808.9846</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B163" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C163">
         <v>33.653759399999998</v>
@@ -7283,13 +8189,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J163">
+        <v>69</v>
+      </c>
+      <c r="K163">
+        <v>41765.555</v>
+      </c>
+      <c r="L163">
+        <v>135.48528999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B164" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C164">
         <v>33.767305999999998</v>
@@ -7315,13 +8230,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J164">
+        <v>12</v>
+      </c>
+      <c r="K164">
+        <v>3325.96</v>
+      </c>
+      <c r="L164">
+        <v>23.562657999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B165" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C165">
         <v>33.826422999999998</v>
@@ -7347,13 +8271,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J165">
+        <v>85</v>
+      </c>
+      <c r="K165">
+        <v>53540.62</v>
+      </c>
+      <c r="L165">
+        <v>166.90216000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B166" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C166">
         <v>33.746398999999997</v>
@@ -7379,13 +8312,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J166">
+        <v>167</v>
+      </c>
+      <c r="K166">
+        <v>94804.22</v>
+      </c>
+      <c r="L166">
+        <v>327.91367000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>330</v>
+        <v>367</v>
       </c>
       <c r="B167" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C167">
         <v>33.7865605</v>
@@ -7411,13 +8353,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J167">
+        <v>5</v>
+      </c>
+      <c r="K167">
+        <v>2267.4456</v>
+      </c>
+      <c r="L167">
+        <v>9.817774</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>332</v>
+        <v>368</v>
       </c>
       <c r="B168" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C168">
         <v>33.807989999999997</v>
@@ -7443,13 +8394,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J168">
+        <v>55</v>
+      </c>
+      <c r="K168">
+        <v>24537.603999999999</v>
+      </c>
+      <c r="L168">
+        <v>107.995514</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B169" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C169">
         <v>33.651388300000001</v>
@@ -7475,13 +8435,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J169">
+        <v>1740</v>
+      </c>
+      <c r="K169">
+        <v>1078862.8</v>
+      </c>
+      <c r="L169">
+        <v>3416.5853999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B170" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C170">
         <v>33.782835599999999</v>
@@ -7507,13 +8476,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J170">
+        <v>180</v>
+      </c>
+      <c r="K170">
+        <v>97480.733999999997</v>
+      </c>
+      <c r="L170">
+        <v>353.43988000000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B171" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C171">
         <v>33.777701800000003</v>
@@ -7539,13 +8517,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J171">
+        <v>865</v>
+      </c>
+      <c r="K171">
+        <v>495516.88</v>
+      </c>
+      <c r="L171">
+        <v>1698.4749999999999</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B172" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C172">
         <v>33.7395864</v>
@@ -7571,13 +8558,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J172">
+        <v>301</v>
+      </c>
+      <c r="K172">
+        <v>183728.2</v>
+      </c>
+      <c r="L172">
+        <v>591.03</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B173" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C173">
         <v>33.923588000000002</v>
@@ -7603,13 +8599,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J173">
+        <v>32</v>
+      </c>
+      <c r="K173">
+        <v>18315.053</v>
+      </c>
+      <c r="L173">
+        <v>62.833754999999996</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B174" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C174">
         <v>33.774696400000003</v>
@@ -7635,13 +8640,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J174">
+        <v>50</v>
+      </c>
+      <c r="K174">
+        <v>23862.947</v>
+      </c>
+      <c r="L174">
+        <v>98.17774</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B175" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C175">
         <v>33.680609699999998</v>
@@ -7667,13 +8681,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J175">
+        <v>321</v>
+      </c>
+      <c r="K175">
+        <v>179966.1</v>
+      </c>
+      <c r="L175">
+        <v>630.30110000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B176" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C176">
         <v>33.9585376</v>
@@ -7699,13 +8722,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J176">
+        <v>59</v>
+      </c>
+      <c r="K176">
+        <v>33332.074000000001</v>
+      </c>
+      <c r="L176">
+        <v>115.84974</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B177" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C177">
         <v>33.950010599999999</v>
@@ -7731,13 +8763,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J177">
+        <v>360</v>
+      </c>
+      <c r="K177">
+        <v>215623.97</v>
+      </c>
+      <c r="L177">
+        <v>706.87976000000003</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B178" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C178">
         <v>33.550077000000002</v>
@@ -7763,13 +8804,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J178">
+        <v>65</v>
+      </c>
+      <c r="K178">
+        <v>23114.36</v>
+      </c>
+      <c r="L178">
+        <v>127.63106500000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B179" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C179">
         <v>33.6102116</v>
@@ -7795,13 +8845,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J179">
+        <v>47</v>
+      </c>
+      <c r="K179">
+        <v>27945.888999999999</v>
+      </c>
+      <c r="L179">
+        <v>92.287080000000003</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B180" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C180">
         <v>33.859588000000002</v>
@@ -7827,13 +8886,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J180">
+        <v>47</v>
+      </c>
+      <c r="K180">
+        <v>27682.567999999999</v>
+      </c>
+      <c r="L180">
+        <v>92.287080000000003</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B181" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C181">
         <v>33.846677</v>
@@ -7859,13 +8927,22 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J181">
+        <v>58</v>
+      </c>
+      <c r="K181">
+        <v>27227.153999999999</v>
+      </c>
+      <c r="L181">
+        <v>113.886185</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B182" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C182">
         <v>33.765948999999999</v>
@@ -7890,6 +8967,15 @@
       <c r="I182" t="str">
         <f>IF(OR(G182 &gt; 0.1, H182 &gt; 0.1), "1", "0")</f>
         <v>0</v>
+      </c>
+      <c r="J182">
+        <v>159</v>
+      </c>
+      <c r="K182">
+        <v>90219.6</v>
+      </c>
+      <c r="L182">
+        <v>312.20522999999997</v>
       </c>
     </row>
   </sheetData>
@@ -7902,7 +8988,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:D2 A7:D55 D3 B4:D4 B5:D5 A6:B6 D6 A57:D64 A56 C56:D56 A66:D99 B65:D65 A154:D178 B153:D153 A101:D152 B100:D100 A180:D182 B179:D179" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:D2 A7:D55 D3 B4:D4 B5:D5 A6:B6 D6 A57:D64 A56 C56:D56 A66:D99 B65:D65 A154:D166 B153:D153 A101:D128 B100:D100 A180:D182 B179:D179 A169:D178 B168:D168 A142:D152 B141:D141 A131:D139 B130:D130 B129:D129 B140:D140 B167:D167" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>